<commit_message>
Where is the sample data?
</commit_message>
<xml_diff>
--- a/outputs/1204var1.xlsx
+++ b/outputs/1204var1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="70">
   <si>
     <t>NAME</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>DISPOSAL ACTION</t>
+  </si>
+  <si>
+    <t>State Revenue Office</t>
   </si>
   <si>
     <t>1204var1</t>
@@ -573,7 +576,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" customWidth="1"/>
     <col min="3" max="3" width="7.28515625" customWidth="1"/>
     <col min="4" max="4" width="357.140625" customWidth="1"/>
@@ -598,325 +601,394 @@
       </c>
     </row>
     <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" t="s">
         <v>24</v>
       </c>
-      <c r="D8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5">
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D21" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D23" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>